<commit_message>
added IO reader for skills file
</commit_message>
<xml_diff>
--- a/data/characters.xlsx
+++ b/data/characters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\PythonProjects\GenshinTeamDPSCalculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2E6C1F-4DB0-47FB-A6EB-22074E7D86B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2E442-09C4-444E-9E0F-CF2735FD9296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1935" windowWidth="23595" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>雷专</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>治疗加成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能等级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9,9,10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -539,43 +551,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="19.125" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="10.25" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="13" max="13" width="10.625" customWidth="1"/>
-    <col min="14" max="14" width="10.375" customWidth="1"/>
-    <col min="16" max="16" width="10.75" customWidth="1"/>
-    <col min="17" max="17" width="10.875" customWidth="1"/>
-    <col min="22" max="22" width="12.75" customWidth="1"/>
-    <col min="24" max="24" width="14.625" customWidth="1"/>
-    <col min="25" max="25" width="10.125" customWidth="1"/>
-    <col min="26" max="26" width="14.625" customWidth="1"/>
-    <col min="27" max="27" width="10.125" customWidth="1"/>
-    <col min="28" max="28" width="14.625" customWidth="1"/>
-    <col min="29" max="29" width="10.125" customWidth="1"/>
-    <col min="30" max="30" width="14.625" customWidth="1"/>
-    <col min="31" max="31" width="10.125" customWidth="1"/>
-    <col min="32" max="32" width="14.625" customWidth="1"/>
-    <col min="33" max="33" width="10.125" customWidth="1"/>
-    <col min="34" max="34" width="14.625" customWidth="1"/>
-    <col min="35" max="35" width="10.125" customWidth="1"/>
-    <col min="36" max="36" width="14.625" customWidth="1"/>
-    <col min="37" max="37" width="10.125" customWidth="1"/>
-    <col min="38" max="38" width="14.625" customWidth="1"/>
-    <col min="39" max="39" width="10.125" customWidth="1"/>
-    <col min="40" max="41" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="10.375" customWidth="1"/>
+    <col min="11" max="11" width="10.25" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="15" max="15" width="10.375" customWidth="1"/>
+    <col min="17" max="17" width="10.75" customWidth="1"/>
+    <col min="18" max="18" width="10.875" customWidth="1"/>
+    <col min="23" max="23" width="12.75" customWidth="1"/>
+    <col min="25" max="25" width="14.625" customWidth="1"/>
+    <col min="26" max="26" width="10.125" customWidth="1"/>
+    <col min="27" max="27" width="14.625" customWidth="1"/>
+    <col min="28" max="28" width="10.125" customWidth="1"/>
+    <col min="29" max="29" width="14.625" customWidth="1"/>
+    <col min="30" max="30" width="10.125" customWidth="1"/>
+    <col min="31" max="31" width="14.625" customWidth="1"/>
+    <col min="32" max="32" width="10.125" customWidth="1"/>
+    <col min="33" max="33" width="14.625" customWidth="1"/>
+    <col min="34" max="34" width="10.125" customWidth="1"/>
+    <col min="35" max="35" width="14.625" customWidth="1"/>
+    <col min="36" max="36" width="10.125" customWidth="1"/>
+    <col min="37" max="37" width="14.625" customWidth="1"/>
+    <col min="38" max="38" width="10.125" customWidth="1"/>
+    <col min="39" max="39" width="14.625" customWidth="1"/>
+    <col min="40" max="40" width="10.125" customWidth="1"/>
+    <col min="41" max="41" width="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -589,141 +602,246 @@
         <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>42</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>44</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>90</v>
+      <c r="C2" t="s">
+        <v>45</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>311</v>
+      </c>
+      <c r="L2">
+        <v>46.6</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>47800</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>65</v>
+      </c>
+      <c r="U2">
+        <v>90</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>51.8</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Building Reaction and UI
</commit_message>
<xml_diff>
--- a/data/characters.xlsx
+++ b/data/characters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\PythonProjects\GenshinTeamDPSCalculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2E442-09C4-444E-9E0F-CF2735FD9296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5C25E3-CC2E-421F-841A-CA2DB035A34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1935" windowWidth="23595" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="23595" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -727,7 +727,7 @@
         <v>45</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
adding ui and exceptions for loading characters and enemy fiels
</commit_message>
<xml_diff>
--- a/data/characters.xlsx
+++ b/data/characters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\PythonProjects\GenshinTeamDPSCalculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5C25E3-CC2E-421F-841A-CA2DB035A34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831D743F-B3D0-40D7-AECB-727F2739931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="23595" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5265" yWindow="3540" windowWidth="25845" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -554,7 +552,7 @@
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding bennet; adding infusion functionality
</commit_message>
<xml_diff>
--- a/data/characters.xlsx
+++ b/data/characters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\PythonProjects\GenshinTeamDPSCalculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831D743F-B3D0-40D7-AECB-727F2739931F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F576A9-F213-404D-841D-E258E73440FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="3540" windowWidth="25845" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>雷专</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -224,6 +216,18 @@
   </si>
   <si>
     <t>9,9,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班尼特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天空之刃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗室</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AP3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -842,6 +846,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implemented Ayaka, BlizzardStrayer, and Mistsplitter
</commit_message>
<xml_diff>
--- a/data/characters.xlsx
+++ b/data/characters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\PythonProjects\GenshinTeamDPSCalculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F576A9-F213-404D-841D-E258E73440FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D446705-E2FE-4931-B610-41319CAEA3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25755" yWindow="2400" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>雷专</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,11 +223,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>天空之刃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>宗室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9,9,9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神里绫华</t>
+  </si>
+  <si>
+    <t>绫华</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰套</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雾切</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天空剑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -553,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:AP4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -768,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>47800</v>
+        <v>4780</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -860,25 +879,25 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>311</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -896,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>4780</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>93.2</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -971,6 +990,134 @@
         <v>0</v>
       </c>
       <c r="AP3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>311</v>
+      </c>
+      <c r="L4">
+        <v>46.6</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>4780</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>40</v>
+      </c>
+      <c r="U4">
+        <v>140</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
         <v>0</v>
       </c>
     </row>

</xml_diff>